<commit_message>
conversão da entrada para csv
</commit_message>
<xml_diff>
--- a/form1/expansao_atualizado_form1.xlsx
+++ b/form1/expansao_atualizado_form1.xlsx
@@ -41,7 +41,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill/>
     </fill>
@@ -104,20 +104,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF6400"/>
-        <bgColor rgb="00FF6400"/>
+        <fgColor rgb="00A020F0"/>
+        <bgColor rgb="00A020F0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00006400"/>
         <bgColor rgb="00006400"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00A020F0"/>
-        <bgColor rgb="00A020F0"/>
       </patternFill>
     </fill>
     <fill>
@@ -153,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -185,16 +179,13 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -575,7 +566,7 @@
     <col width="8" customWidth="1" min="3" max="3"/>
     <col width="52" customWidth="1" min="4" max="4"/>
     <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="39" customWidth="1" min="6" max="6"/>
+    <col width="51" customWidth="1" min="6" max="6"/>
     <col width="27" customWidth="1" min="7" max="7"/>
     <col width="151" customWidth="1" min="8" max="8"/>
     <col width="34" customWidth="1" min="9" max="9"/>
@@ -663,10 +654,14 @@
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t>Atrasado</t>
-        </is>
-      </c>
-      <c r="F2" s="3" t="n"/>
+          <t>Envio Duplicado</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>01/04/2025, 02/04/2025, 06/04/2025, 09/04/2025</t>
+        </is>
+      </c>
       <c r="G2" s="5" t="inlineStr">
         <is>
           <t>Não</t>
@@ -894,7 +889,7 @@
           <t>Daniele de Souza Lima Mei</t>
         </is>
       </c>
-      <c r="E7" s="11" t="inlineStr">
+      <c r="E7" s="4" t="inlineStr">
         <is>
           <t>Envio Duplicado</t>
         </is>
@@ -992,14 +987,14 @@
           <t>Danielli Casarin Vilela de Almeida Cansian</t>
         </is>
       </c>
-      <c r="E9" s="6" t="inlineStr">
-        <is>
-          <t>Enviado</t>
+      <c r="E9" s="4" t="inlineStr">
+        <is>
+          <t>Envio Duplicado</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>21/03/2025</t>
+          <t>20/03/2025, 21/03/2025</t>
         </is>
       </c>
       <c r="G9" s="7" t="inlineStr">
@@ -1025,7 +1020,7 @@
       <c r="K9" s="3" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="12" t="inlineStr">
+      <c r="A10" s="11" t="inlineStr">
         <is>
           <t>Curitiba</t>
         </is>
@@ -1070,7 +1065,7 @@
       <c r="K10" s="3" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="12" t="inlineStr">
+      <c r="A11" s="11" t="inlineStr">
         <is>
           <t>Curitiba</t>
         </is>
@@ -1115,7 +1110,7 @@
       <c r="K11" s="3" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="12" t="inlineStr">
+      <c r="A12" s="11" t="inlineStr">
         <is>
           <t>Curitiba</t>
         </is>
@@ -1160,7 +1155,7 @@
       <c r="K12" s="3" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="12" t="inlineStr">
+      <c r="A13" s="11" t="inlineStr">
         <is>
           <t>Curitiba</t>
         </is>
@@ -1205,7 +1200,7 @@
       <c r="K13" s="3" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="12" t="inlineStr">
+      <c r="A14" s="11" t="inlineStr">
         <is>
           <t>Curitiba</t>
         </is>
@@ -1250,7 +1245,7 @@
       <c r="K14" s="3" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="12" t="inlineStr">
+      <c r="A15" s="11" t="inlineStr">
         <is>
           <t>Curitiba</t>
         </is>
@@ -1340,7 +1335,7 @@
       <c r="K16" s="3" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="12" t="inlineStr">
+      <c r="A17" s="11" t="inlineStr">
         <is>
           <t>Curitiba</t>
         </is>
@@ -1430,7 +1425,7 @@
       <c r="K18" s="3" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="13" t="inlineStr">
+      <c r="A19" s="12" t="inlineStr">
         <is>
           <t>Guarapuava</t>
         </is>
@@ -1446,7 +1441,7 @@
         </is>
       </c>
       <c r="D19" s="3" t="n"/>
-      <c r="E19" s="14" t="inlineStr">
+      <c r="E19" s="13" t="inlineStr">
         <is>
           <t>Sem Técnico</t>
         </is>
@@ -1692,7 +1687,7 @@
       <c r="K24" s="3" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="13" t="inlineStr">
+      <c r="A25" s="12" t="inlineStr">
         <is>
           <t>Guarapuava</t>
         </is>
@@ -1966,7 +1961,7 @@
       <c r="K30" s="3" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="12" t="inlineStr">
+      <c r="A31" s="11" t="inlineStr">
         <is>
           <t>Curitiba</t>
         </is>
@@ -2011,7 +2006,7 @@
       <c r="K31" s="3" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="13" t="inlineStr">
+      <c r="A32" s="12" t="inlineStr">
         <is>
           <t>Guarapuava</t>
         </is>
@@ -2076,7 +2071,7 @@
           <t>Gislaine Souza Rosa</t>
         </is>
       </c>
-      <c r="E33" s="11" t="inlineStr">
+      <c r="E33" s="4" t="inlineStr">
         <is>
           <t>Envio Duplicado</t>
         </is>
@@ -2199,7 +2194,7 @@
       <c r="K35" s="3" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="13" t="inlineStr">
+      <c r="A36" s="12" t="inlineStr">
         <is>
           <t>Guarapuava</t>
         </is>
@@ -2334,7 +2329,7 @@
       <c r="K38" s="3" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="13" t="inlineStr">
+      <c r="A39" s="12" t="inlineStr">
         <is>
           <t>Guarapuava</t>
         </is>
@@ -2354,14 +2349,14 @@
           <t>Aramis Vinicius de Paula Oliveira</t>
         </is>
       </c>
-      <c r="E39" s="6" t="inlineStr">
-        <is>
-          <t>Enviado</t>
+      <c r="E39" s="4" t="inlineStr">
+        <is>
+          <t>Envio Duplicado</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>21/03/2025</t>
+          <t>19/03/2025, 21/03/2025</t>
         </is>
       </c>
       <c r="G39" s="5" t="inlineStr">
@@ -2559,7 +2554,7 @@
       <c r="K43" s="3" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="13" t="inlineStr">
+      <c r="A44" s="12" t="inlineStr">
         <is>
           <t>Guarapuava</t>
         </is>
@@ -2649,7 +2644,7 @@
       <c r="K45" s="3" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="12" t="inlineStr">
+      <c r="A46" s="11" t="inlineStr">
         <is>
           <t>Curitiba</t>
         </is>
@@ -2669,7 +2664,7 @@
           <t>João Henrique Assunção de Sousa</t>
         </is>
       </c>
-      <c r="E46" s="14" t="inlineStr">
+      <c r="E46" s="13" t="inlineStr">
         <is>
           <t>Sem Técnico</t>
         </is>
@@ -2690,7 +2685,7 @@
       <c r="K46" s="3" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="12" t="inlineStr">
+      <c r="A47" s="11" t="inlineStr">
         <is>
           <t>Curitiba</t>
         </is>
@@ -2710,7 +2705,7 @@
           <t>João Henrique Assunção de Sousa</t>
         </is>
       </c>
-      <c r="E47" s="14" t="inlineStr">
+      <c r="E47" s="13" t="inlineStr">
         <is>
           <t>Sem Técnico</t>
         </is>
@@ -2731,7 +2726,7 @@
       <c r="K47" s="3" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="12" t="inlineStr">
+      <c r="A48" s="11" t="inlineStr">
         <is>
           <t>Curitiba</t>
         </is>
@@ -2751,7 +2746,7 @@
           <t>Jean Eriksen de Miranda</t>
         </is>
       </c>
-      <c r="E48" s="11" t="inlineStr">
+      <c r="E48" s="4" t="inlineStr">
         <is>
           <t>Envio Duplicado</t>
         </is>
@@ -2804,12 +2799,16 @@
           <t>Moacir Roberto Heimann</t>
         </is>
       </c>
-      <c r="E49" s="14" t="inlineStr">
-        <is>
-          <t>Sem Técnico</t>
-        </is>
-      </c>
-      <c r="F49" s="3" t="n"/>
+      <c r="E49" s="6" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F49" s="3" t="inlineStr">
+        <is>
+          <t>14/04/2025</t>
+        </is>
+      </c>
       <c r="G49" s="5" t="inlineStr">
         <is>
           <t>Não</t>
@@ -2825,7 +2824,7 @@
       <c r="K49" s="3" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="13" t="inlineStr">
+      <c r="A50" s="12" t="inlineStr">
         <is>
           <t>Guarapuava</t>
         </is>
@@ -2845,7 +2844,7 @@
           <t>Vilmar Ribeiro</t>
         </is>
       </c>
-      <c r="E50" s="11" t="inlineStr">
+      <c r="E50" s="4" t="inlineStr">
         <is>
           <t>Envio Duplicado</t>
         </is>
@@ -3013,7 +3012,7 @@
       <c r="K53" s="3" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="13" t="inlineStr">
+      <c r="A54" s="12" t="inlineStr">
         <is>
           <t>Guarapuava</t>
         </is>
@@ -3029,7 +3028,7 @@
         </is>
       </c>
       <c r="D54" s="3" t="n"/>
-      <c r="E54" s="14" t="inlineStr">
+      <c r="E54" s="13" t="inlineStr">
         <is>
           <t>Sem Técnico</t>
         </is>
@@ -3070,12 +3069,16 @@
           <t>Eliane Stefani Dantas Dias</t>
         </is>
       </c>
-      <c r="E55" s="14" t="inlineStr">
-        <is>
-          <t>Sem Técnico</t>
-        </is>
-      </c>
-      <c r="F55" s="3" t="n"/>
+      <c r="E55" s="4" t="inlineStr">
+        <is>
+          <t>Envio Duplicado</t>
+        </is>
+      </c>
+      <c r="F55" s="3" t="inlineStr">
+        <is>
+          <t>28/03/2025, 28/03/2025</t>
+        </is>
+      </c>
       <c r="G55" s="5" t="inlineStr">
         <is>
           <t>Não</t>
@@ -3136,7 +3139,7 @@
       <c r="K56" s="3" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="12" t="inlineStr">
+      <c r="A57" s="11" t="inlineStr">
         <is>
           <t>Curitiba</t>
         </is>
@@ -3181,7 +3184,7 @@
       <c r="K57" s="3" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="12" t="inlineStr">
+      <c r="A58" s="11" t="inlineStr">
         <is>
           <t>Curitiba</t>
         </is>
@@ -3201,7 +3204,7 @@
           <t>Adriano Campos Chagas</t>
         </is>
       </c>
-      <c r="E58" s="11" t="inlineStr">
+      <c r="E58" s="4" t="inlineStr">
         <is>
           <t>Envio Duplicado</t>
         </is>

</xml_diff>